<commit_message>
updated CCS vars and ETS
</commit_message>
<xml_diff>
--- a/InputData/ccs/BFoCPAbS/BAU Fraction of CCS Potential Achieved by Sector.xlsx
+++ b/InputData/ccs/BFoCPAbS/BAU Fraction of CCS Potential Achieved by Sector.xlsx
@@ -1,28 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\Documents\Energy Policy Simulator\Models\eps-eu\InputData\ccs\BFoCPAbS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\EU\EU-EPS\InputData\ccs\BFoCPAbS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6291ED8-88B7-400E-8BC8-8880252CCA87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107A75E9-78A6-4B3A-BBC7-9D6873899BB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12090" yWindow="-16320" windowWidth="18945" windowHeight="11745" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11280" yWindow="2805" windowWidth="14460" windowHeight="13020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BFoCPAbS-electricity" sheetId="12" r:id="rId2"/>
     <sheet name="BFoCPAbS-industry" sheetId="13" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
   <si>
     <t>Source:</t>
   </si>
@@ -108,28 +119,79 @@
     <t>municipal solid waste</t>
   </si>
   <si>
-    <t>cement and other carbonates</t>
+    <t>agriculture and forestry 01T03</t>
   </si>
   <si>
-    <t>natural gas and petroleum systems</t>
+    <t>coal mining 05</t>
   </si>
   <si>
-    <t>iron and steel</t>
+    <t>oil and gas extraction 06</t>
   </si>
   <si>
-    <t>chemicals</t>
+    <t>other mining and quarrying 07T08</t>
   </si>
   <si>
-    <t>coal mining</t>
+    <t>food beverage and tobacco 10T12</t>
   </si>
   <si>
-    <t>waste management</t>
+    <t>textiles apparel and leather 13T15</t>
   </si>
   <si>
-    <t>agriculture</t>
+    <t>wood products 16</t>
   </si>
   <si>
-    <t>other industries</t>
+    <t>pulp paper and printing 17T18</t>
+  </si>
+  <si>
+    <t>refined petroleum and coke 19</t>
+  </si>
+  <si>
+    <t>chemicals 20</t>
+  </si>
+  <si>
+    <t>rubber and plastic products 22</t>
+  </si>
+  <si>
+    <t>glass and glass products 231</t>
+  </si>
+  <si>
+    <t>cement and other nonmetallic minerals 239</t>
+  </si>
+  <si>
+    <t>iron and steel 241</t>
+  </si>
+  <si>
+    <t>other metals 242</t>
+  </si>
+  <si>
+    <t>metal products except machinery and vehicles 25</t>
+  </si>
+  <si>
+    <t>computers and electronics 26</t>
+  </si>
+  <si>
+    <t>appliances and electrical equipment 27</t>
+  </si>
+  <si>
+    <t>other machinery 28</t>
+  </si>
+  <si>
+    <t>road vehicles 29</t>
+  </si>
+  <si>
+    <t>nonroad vehicles 30</t>
+  </si>
+  <si>
+    <t>other manufacturing 31T33</t>
+  </si>
+  <si>
+    <t>energy pipelines and gas processing 352T353</t>
+  </si>
+  <si>
+    <t>water and waste 36T39</t>
+  </si>
+  <si>
+    <t>construction 41T43</t>
   </si>
 </sst>
 </file>
@@ -548,20 +610,20 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="103.46484375" customWidth="1"/>
-    <col min="3" max="3" width="17.19921875" customWidth="1"/>
-    <col min="4" max="4" width="22.19921875" customWidth="1"/>
-    <col min="5" max="5" width="18.46484375" customWidth="1"/>
+    <col min="2" max="2" width="103.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -569,83 +631,83 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
       <c r="D20" s="5"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
     </row>
@@ -664,12 +726,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.796875" customWidth="1"/>
+    <col min="1" max="1" width="44.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>11</v>
       </c>
@@ -773,7 +835,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -877,7 +939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>13</v>
       </c>
@@ -981,7 +1043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>14</v>
       </c>
@@ -1085,7 +1147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>15</v>
       </c>
@@ -1189,7 +1251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>16</v>
       </c>
@@ -1293,7 +1355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -1397,7 +1459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>18</v>
       </c>
@@ -1501,7 +1563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -1605,7 +1667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>20</v>
       </c>
@@ -1709,7 +1771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1813,7 +1875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1917,7 +1979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -2021,7 +2083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>24</v>
       </c>
@@ -2125,7 +2187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -2229,7 +2291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -2333,7 +2395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -2448,18 +2510,16 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:AG9"/>
+  <dimension ref="A1:AG27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>11</v>
       </c>
@@ -2560,811 +2620,2629 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>28</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
-      <c r="AA2">
-        <v>0</v>
-      </c>
-      <c r="AB2">
-        <v>0</v>
-      </c>
-      <c r="AC2">
-        <v>0</v>
-      </c>
-      <c r="AD2">
-        <v>0</v>
-      </c>
-      <c r="AE2">
-        <v>0</v>
-      </c>
-      <c r="AF2">
-        <v>0</v>
-      </c>
-      <c r="AG2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>29</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
-      <c r="W3">
-        <v>0</v>
-      </c>
-      <c r="X3">
-        <v>0</v>
-      </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
-      <c r="Z3">
-        <v>0</v>
-      </c>
-      <c r="AA3">
-        <v>0</v>
-      </c>
-      <c r="AB3">
-        <v>0</v>
-      </c>
-      <c r="AC3">
-        <v>0</v>
-      </c>
-      <c r="AD3">
-        <v>0</v>
-      </c>
-      <c r="AE3">
-        <v>0</v>
-      </c>
-      <c r="AF3">
-        <v>0</v>
-      </c>
-      <c r="AG3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>30</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-      <c r="Y4">
-        <v>0</v>
-      </c>
-      <c r="Z4">
-        <v>0</v>
-      </c>
-      <c r="AA4">
-        <v>0</v>
-      </c>
-      <c r="AB4">
-        <v>0</v>
-      </c>
-      <c r="AC4">
-        <v>0</v>
-      </c>
-      <c r="AD4">
-        <v>0</v>
-      </c>
-      <c r="AE4">
-        <v>0</v>
-      </c>
-      <c r="AF4">
-        <v>0</v>
-      </c>
-      <c r="AG4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>31</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>0</v>
-      </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
-      <c r="Y5">
-        <v>0</v>
-      </c>
-      <c r="Z5">
-        <v>0</v>
-      </c>
-      <c r="AA5">
-        <v>0</v>
-      </c>
-      <c r="AB5">
-        <v>0</v>
-      </c>
-      <c r="AC5">
-        <v>0</v>
-      </c>
-      <c r="AD5">
-        <v>0</v>
-      </c>
-      <c r="AE5">
-        <v>0</v>
-      </c>
-      <c r="AF5">
-        <v>0</v>
-      </c>
-      <c r="AG5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <v>0</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>32</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="V6">
-        <v>0</v>
-      </c>
-      <c r="W6">
-        <v>0</v>
-      </c>
-      <c r="X6">
-        <v>0</v>
-      </c>
-      <c r="Y6">
-        <v>0</v>
-      </c>
-      <c r="Z6">
-        <v>0</v>
-      </c>
-      <c r="AA6">
-        <v>0</v>
-      </c>
-      <c r="AB6">
-        <v>0</v>
-      </c>
-      <c r="AC6">
-        <v>0</v>
-      </c>
-      <c r="AD6">
-        <v>0</v>
-      </c>
-      <c r="AE6">
-        <v>0</v>
-      </c>
-      <c r="AF6">
-        <v>0</v>
-      </c>
-      <c r="AG6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+      <c r="AG7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>33</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-      <c r="V7">
-        <v>0</v>
-      </c>
-      <c r="W7">
-        <v>0</v>
-      </c>
-      <c r="X7">
-        <v>0</v>
-      </c>
-      <c r="Y7">
-        <v>0</v>
-      </c>
-      <c r="Z7">
-        <v>0</v>
-      </c>
-      <c r="AA7">
-        <v>0</v>
-      </c>
-      <c r="AB7">
-        <v>0</v>
-      </c>
-      <c r="AC7">
-        <v>0</v>
-      </c>
-      <c r="AD7">
-        <v>0</v>
-      </c>
-      <c r="AE7">
-        <v>0</v>
-      </c>
-      <c r="AF7">
-        <v>0</v>
-      </c>
-      <c r="AG7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
+      <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>34</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
-      <c r="V8">
-        <v>0</v>
-      </c>
-      <c r="W8">
-        <v>0</v>
-      </c>
-      <c r="X8">
-        <v>0</v>
-      </c>
-      <c r="Y8">
-        <v>0</v>
-      </c>
-      <c r="Z8">
-        <v>0</v>
-      </c>
-      <c r="AA8">
-        <v>0</v>
-      </c>
-      <c r="AB8">
-        <v>0</v>
-      </c>
-      <c r="AC8">
-        <v>0</v>
-      </c>
-      <c r="AD8">
-        <v>0</v>
-      </c>
-      <c r="AE8">
-        <v>0</v>
-      </c>
-      <c r="AF8">
-        <v>0</v>
-      </c>
-      <c r="AG8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>35</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-      <c r="T9">
-        <v>0</v>
-      </c>
-      <c r="U9">
-        <v>0</v>
-      </c>
-      <c r="V9">
-        <v>0</v>
-      </c>
-      <c r="W9">
-        <v>0</v>
-      </c>
-      <c r="X9">
-        <v>0</v>
-      </c>
-      <c r="Y9">
-        <v>0</v>
-      </c>
-      <c r="Z9">
-        <v>0</v>
-      </c>
-      <c r="AA9">
-        <v>0</v>
-      </c>
-      <c r="AB9">
-        <v>0</v>
-      </c>
-      <c r="AC9">
-        <v>0</v>
-      </c>
-      <c r="AD9">
-        <v>0</v>
-      </c>
-      <c r="AE9">
-        <v>0</v>
-      </c>
-      <c r="AF9">
-        <v>0</v>
-      </c>
-      <c r="AG9">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <v>0</v>
+      </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>0</v>
+      </c>
+      <c r="AF10">
+        <v>0</v>
+      </c>
+      <c r="AG10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AE11">
+        <v>0</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AC12">
+        <v>0</v>
+      </c>
+      <c r="AD12">
+        <v>0</v>
+      </c>
+      <c r="AE12">
+        <v>0</v>
+      </c>
+      <c r="AF12">
+        <v>0</v>
+      </c>
+      <c r="AG12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
+      <c r="AA13">
+        <v>0</v>
+      </c>
+      <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AC13">
+        <v>0</v>
+      </c>
+      <c r="AD13">
+        <v>0</v>
+      </c>
+      <c r="AE13">
+        <v>0</v>
+      </c>
+      <c r="AF13">
+        <v>0</v>
+      </c>
+      <c r="AG13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <v>0</v>
+      </c>
+      <c r="AB14">
+        <v>0</v>
+      </c>
+      <c r="AC14">
+        <v>0</v>
+      </c>
+      <c r="AD14">
+        <v>0</v>
+      </c>
+      <c r="AE14">
+        <v>0</v>
+      </c>
+      <c r="AF14">
+        <v>0</v>
+      </c>
+      <c r="AG14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <v>0</v>
+      </c>
+      <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15">
+        <v>0</v>
+      </c>
+      <c r="AD15">
+        <v>0</v>
+      </c>
+      <c r="AE15">
+        <v>0</v>
+      </c>
+      <c r="AF15">
+        <v>0</v>
+      </c>
+      <c r="AG15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
+      <c r="AA16">
+        <v>0</v>
+      </c>
+      <c r="AB16">
+        <v>0</v>
+      </c>
+      <c r="AC16">
+        <v>0</v>
+      </c>
+      <c r="AD16">
+        <v>0</v>
+      </c>
+      <c r="AE16">
+        <v>0</v>
+      </c>
+      <c r="AF16">
+        <v>0</v>
+      </c>
+      <c r="AG16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17">
+        <v>0</v>
+      </c>
+      <c r="AA17">
+        <v>0</v>
+      </c>
+      <c r="AB17">
+        <v>0</v>
+      </c>
+      <c r="AC17">
+        <v>0</v>
+      </c>
+      <c r="AD17">
+        <v>0</v>
+      </c>
+      <c r="AE17">
+        <v>0</v>
+      </c>
+      <c r="AF17">
+        <v>0</v>
+      </c>
+      <c r="AG17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <v>0</v>
+      </c>
+      <c r="Z18">
+        <v>0</v>
+      </c>
+      <c r="AA18">
+        <v>0</v>
+      </c>
+      <c r="AB18">
+        <v>0</v>
+      </c>
+      <c r="AC18">
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <v>0</v>
+      </c>
+      <c r="AE18">
+        <v>0</v>
+      </c>
+      <c r="AF18">
+        <v>0</v>
+      </c>
+      <c r="AG18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <v>0</v>
+      </c>
+      <c r="AA19">
+        <v>0</v>
+      </c>
+      <c r="AB19">
+        <v>0</v>
+      </c>
+      <c r="AC19">
+        <v>0</v>
+      </c>
+      <c r="AD19">
+        <v>0</v>
+      </c>
+      <c r="AE19">
+        <v>0</v>
+      </c>
+      <c r="AF19">
+        <v>0</v>
+      </c>
+      <c r="AG19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>0</v>
+      </c>
+      <c r="X20">
+        <v>0</v>
+      </c>
+      <c r="Y20">
+        <v>0</v>
+      </c>
+      <c r="Z20">
+        <v>0</v>
+      </c>
+      <c r="AA20">
+        <v>0</v>
+      </c>
+      <c r="AB20">
+        <v>0</v>
+      </c>
+      <c r="AC20">
+        <v>0</v>
+      </c>
+      <c r="AD20">
+        <v>0</v>
+      </c>
+      <c r="AE20">
+        <v>0</v>
+      </c>
+      <c r="AF20">
+        <v>0</v>
+      </c>
+      <c r="AG20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+      <c r="Y21">
+        <v>0</v>
+      </c>
+      <c r="Z21">
+        <v>0</v>
+      </c>
+      <c r="AA21">
+        <v>0</v>
+      </c>
+      <c r="AB21">
+        <v>0</v>
+      </c>
+      <c r="AC21">
+        <v>0</v>
+      </c>
+      <c r="AD21">
+        <v>0</v>
+      </c>
+      <c r="AE21">
+        <v>0</v>
+      </c>
+      <c r="AF21">
+        <v>0</v>
+      </c>
+      <c r="AG21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+      <c r="X22">
+        <v>0</v>
+      </c>
+      <c r="Y22">
+        <v>0</v>
+      </c>
+      <c r="Z22">
+        <v>0</v>
+      </c>
+      <c r="AA22">
+        <v>0</v>
+      </c>
+      <c r="AB22">
+        <v>0</v>
+      </c>
+      <c r="AC22">
+        <v>0</v>
+      </c>
+      <c r="AD22">
+        <v>0</v>
+      </c>
+      <c r="AE22">
+        <v>0</v>
+      </c>
+      <c r="AF22">
+        <v>0</v>
+      </c>
+      <c r="AG22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
+      <c r="Y23">
+        <v>0</v>
+      </c>
+      <c r="Z23">
+        <v>0</v>
+      </c>
+      <c r="AA23">
+        <v>0</v>
+      </c>
+      <c r="AB23">
+        <v>0</v>
+      </c>
+      <c r="AC23">
+        <v>0</v>
+      </c>
+      <c r="AD23">
+        <v>0</v>
+      </c>
+      <c r="AE23">
+        <v>0</v>
+      </c>
+      <c r="AF23">
+        <v>0</v>
+      </c>
+      <c r="AG23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <v>0</v>
+      </c>
+      <c r="X24">
+        <v>0</v>
+      </c>
+      <c r="Y24">
+        <v>0</v>
+      </c>
+      <c r="Z24">
+        <v>0</v>
+      </c>
+      <c r="AA24">
+        <v>0</v>
+      </c>
+      <c r="AB24">
+        <v>0</v>
+      </c>
+      <c r="AC24">
+        <v>0</v>
+      </c>
+      <c r="AD24">
+        <v>0</v>
+      </c>
+      <c r="AE24">
+        <v>0</v>
+      </c>
+      <c r="AF24">
+        <v>0</v>
+      </c>
+      <c r="AG24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <v>0</v>
+      </c>
+      <c r="X25">
+        <v>0</v>
+      </c>
+      <c r="Y25">
+        <v>0</v>
+      </c>
+      <c r="Z25">
+        <v>0</v>
+      </c>
+      <c r="AA25">
+        <v>0</v>
+      </c>
+      <c r="AB25">
+        <v>0</v>
+      </c>
+      <c r="AC25">
+        <v>0</v>
+      </c>
+      <c r="AD25">
+        <v>0</v>
+      </c>
+      <c r="AE25">
+        <v>0</v>
+      </c>
+      <c r="AF25">
+        <v>0</v>
+      </c>
+      <c r="AG25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <v>0</v>
+      </c>
+      <c r="W26">
+        <v>0</v>
+      </c>
+      <c r="X26">
+        <v>0</v>
+      </c>
+      <c r="Y26">
+        <v>0</v>
+      </c>
+      <c r="Z26">
+        <v>0</v>
+      </c>
+      <c r="AA26">
+        <v>0</v>
+      </c>
+      <c r="AB26">
+        <v>0</v>
+      </c>
+      <c r="AC26">
+        <v>0</v>
+      </c>
+      <c r="AD26">
+        <v>0</v>
+      </c>
+      <c r="AE26">
+        <v>0</v>
+      </c>
+      <c r="AF26">
+        <v>0</v>
+      </c>
+      <c r="AG26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+      <c r="Y27">
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <v>0</v>
+      </c>
+      <c r="AA27">
+        <v>0</v>
+      </c>
+      <c r="AB27">
+        <v>0</v>
+      </c>
+      <c r="AC27">
+        <v>0</v>
+      </c>
+      <c r="AD27">
+        <v>0</v>
+      </c>
+      <c r="AE27">
+        <v>0</v>
+      </c>
+      <c r="AF27">
+        <v>0</v>
+      </c>
+      <c r="AG27">
         <v>0</v>
       </c>
     </row>

</xml_diff>